<commit_message>
update data types where needed
</commit_message>
<xml_diff>
--- a/data_final/dictionaries/S_Dict.xlsx
+++ b/data_final/dictionaries/S_Dict.xlsx
@@ -196,6 +196,9 @@
     <t xml:space="preserve">BE01</t>
   </si>
   <si>
+    <t xml:space="preserve">Float</t>
+  </si>
+  <si>
     <t xml:space="preserve">1980, 1990, and 2000 data from respective decennial censuses downloaded from Social Explorer at county level and aggregated upwards.</t>
   </si>
   <si>
@@ -218,9 +221,6 @@
   </si>
   <si>
     <t xml:space="preserve">https://github.com/GeoDaCenter/opioid-policy-scan/blob/main/data_final/metadata/Race_Ethnicity_2018.md</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Float</t>
   </si>
   <si>
     <t xml:space="preserve">BlackP</t>
@@ -1110,13 +1110,13 @@
     <t xml:space="preserve">Mean yearly Hepatitis C cases in people over 75 years of age from 2013-2016</t>
   </si>
   <si>
-    <t xml:space="preserve">blkHcv</t>
+    <t xml:space="preserve">BlkHcv</t>
   </si>
   <si>
     <t xml:space="preserve">Mean yearly Hepatitis C cases in populations identified as non-hispanic Black alone across 2013-2016</t>
   </si>
   <si>
-    <t xml:space="preserve">nonBlkHcv</t>
+    <t xml:space="preserve">NonBlkHcv</t>
   </si>
   <si>
     <t xml:space="preserve">Mean yearly Hepatitis C cases in populations non-Black other race/ethnicity populations 2013-2016</t>
@@ -2129,8 +2129,8 @@
   </sheetPr>
   <dimension ref="A1:R232"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K35" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N49" activeCellId="0" sqref="N49"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L87" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N106" activeCellId="0" sqref="N106:N107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2545,14 +2545,14 @@
         <v>57</v>
       </c>
       <c r="N9" s="6" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="O9" s="6" t="n">
         <v>3064381</v>
       </c>
       <c r="P9" s="6"/>
       <c r="Q9" s="6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2563,13 +2563,13 @@
         <v>14</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="K10" s="6" t="s">
         <v>43</v>
@@ -2578,7 +2578,7 @@
         <v>44</v>
       </c>
       <c r="M10" s="6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="N10" s="6" t="s">
         <v>38</v>
@@ -2612,13 +2612,13 @@
         <v>14</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K11" s="6" t="s">
         <v>35</v>
@@ -2630,7 +2630,7 @@
         <v>37</v>
       </c>
       <c r="N11" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O11" s="6" t="n">
         <v>76.03</v>
@@ -2669,7 +2669,7 @@
         <v>68</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K12" s="6" t="s">
         <v>35</v>
@@ -2681,7 +2681,7 @@
         <v>37</v>
       </c>
       <c r="N12" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O12" s="6" t="n">
         <v>3.7</v>
@@ -2720,7 +2720,7 @@
         <v>70</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K13" s="6" t="s">
         <v>35</v>
@@ -2732,7 +2732,7 @@
         <v>37</v>
       </c>
       <c r="N13" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O13" s="6" t="n">
         <v>1.3</v>
@@ -2771,7 +2771,7 @@
         <v>72</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K14" s="6" t="s">
         <v>35</v>
@@ -2783,7 +2783,7 @@
         <v>37</v>
       </c>
       <c r="N14" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O14" s="6" t="n">
         <v>8.33</v>
@@ -2822,7 +2822,7 @@
         <v>74</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K15" s="6" t="s">
         <v>35</v>
@@ -2834,7 +2834,7 @@
         <v>37</v>
       </c>
       <c r="N15" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O15" s="6" t="n">
         <v>0.66</v>
@@ -2873,7 +2873,7 @@
         <v>76</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K16" s="6" t="s">
         <v>35</v>
@@ -2885,7 +2885,7 @@
         <v>37</v>
       </c>
       <c r="N16" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O16" s="6" t="n">
         <v>9.98</v>
@@ -2924,7 +2924,7 @@
         <v>78</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K17" s="6" t="s">
         <v>35</v>
@@ -2936,7 +2936,7 @@
         <v>37</v>
       </c>
       <c r="N17" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O17" s="6" t="n">
         <v>12.5</v>
@@ -2982,7 +2982,7 @@
       </c>
       <c r="M18" s="6"/>
       <c r="N18" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O18" s="6" t="n">
         <v>78</v>
@@ -3033,7 +3033,7 @@
         <v>37</v>
       </c>
       <c r="N19" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O19" s="6" t="n">
         <v>12.74</v>
@@ -3084,7 +3084,7 @@
         <v>37</v>
       </c>
       <c r="N20" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O20" s="6" t="n">
         <v>59.43</v>
@@ -3135,7 +3135,7 @@
         <v>37</v>
       </c>
       <c r="N21" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O21" s="6" t="n">
         <v>14.72</v>
@@ -3186,7 +3186,7 @@
         <v>37</v>
       </c>
       <c r="N22" s="6" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="O22" s="6" t="n">
         <v>453008</v>
@@ -3237,7 +3237,7 @@
         <v>37</v>
       </c>
       <c r="N23" s="6" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="O23" s="6" t="n">
         <v>909873</v>
@@ -3288,7 +3288,7 @@
         <v>37</v>
       </c>
       <c r="N24" s="6" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="O24" s="6" t="n">
         <v>444352</v>
@@ -3339,7 +3339,7 @@
         <v>37</v>
       </c>
       <c r="N25" s="6" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="O25" s="6" t="n">
         <v>485160</v>
@@ -3390,7 +3390,7 @@
         <v>37</v>
       </c>
       <c r="N26" s="6" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="O26" s="6" t="n">
         <v>2972063</v>
@@ -3426,7 +3426,7 @@
         <v>37</v>
       </c>
       <c r="N27" s="6" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="O27" s="1" t="n">
         <v>2359934</v>
@@ -3471,7 +3471,7 @@
         <v>37</v>
       </c>
       <c r="N28" s="6" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="O28" s="6" t="n">
         <v>467768</v>
@@ -3516,7 +3516,7 @@
         <v>37</v>
       </c>
       <c r="N29" s="6" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="O29" s="6" t="n">
         <v>476486</v>
@@ -3567,7 +3567,7 @@
         <v>37</v>
       </c>
       <c r="N30" s="6" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="O30" s="6" t="n">
         <v>487173</v>
@@ -3618,7 +3618,7 @@
         <v>37</v>
       </c>
       <c r="N31" s="6" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="O31" s="6" t="n">
         <v>454466</v>
@@ -3669,7 +3669,7 @@
         <v>37</v>
       </c>
       <c r="N32" s="6" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="O32" s="6" t="n">
         <v>1073499</v>
@@ -3708,7 +3708,7 @@
         <v>37</v>
       </c>
       <c r="N33" s="6" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="O33" s="6" t="n">
         <v>5661461</v>
@@ -3754,7 +3754,7 @@
         <v>37</v>
       </c>
       <c r="N34" s="6" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="O34" s="6" t="n">
         <v>4587962</v>
@@ -3796,7 +3796,7 @@
         <v>37</v>
       </c>
       <c r="N35" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O35" s="6" t="n">
         <v>12.7</v>
@@ -3847,7 +3847,7 @@
         <v>37</v>
       </c>
       <c r="N36" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O36" s="6" t="n">
         <v>8.89</v>
@@ -3886,7 +3886,7 @@
         <v>51</v>
       </c>
       <c r="N37" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O37" s="6" t="n">
         <v>9.58</v>
@@ -3920,7 +3920,7 @@
         <v>45</v>
       </c>
       <c r="N38" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O38" s="6" t="n">
         <v>3.35</v>
@@ -3954,7 +3954,7 @@
         <v>45</v>
       </c>
       <c r="N39" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O39" s="6" t="n">
         <v>25.61</v>
@@ -4111,7 +4111,7 @@
         <v>150</v>
       </c>
       <c r="N43" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O43" s="6" t="n">
         <v>5.3</v>
@@ -4162,7 +4162,7 @@
         <v>150</v>
       </c>
       <c r="N44" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O44" s="6" t="n">
         <v>11.5</v>
@@ -4270,7 +4270,7 @@
         <v>162</v>
       </c>
       <c r="N47" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O47" s="6" t="n">
         <v>5.53</v>
@@ -4308,7 +4308,7 @@
         <v>162</v>
       </c>
       <c r="N48" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O48" s="6" t="n">
         <v>48.09</v>
@@ -4347,7 +4347,7 @@
       </c>
       <c r="M49" s="6"/>
       <c r="N49" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O49" s="6" t="n">
         <v>0.46</v>
@@ -4369,7 +4369,7 @@
         <v>170</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="K50" s="6" t="s">
         <v>43</v>
@@ -4378,10 +4378,10 @@
         <v>44</v>
       </c>
       <c r="M50" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="N50" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O50" s="6" t="n">
         <v>8.44</v>
@@ -4405,7 +4405,7 @@
         <v>173</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="K51" s="6" t="s">
         <v>43</v>
@@ -4414,10 +4414,10 @@
         <v>44</v>
       </c>
       <c r="M51" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="N51" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O51" s="6" t="n">
         <v>20</v>
@@ -4441,7 +4441,7 @@
         <v>175</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="K52" s="6" t="s">
         <v>43</v>
@@ -4450,10 +4450,10 @@
         <v>44</v>
       </c>
       <c r="M52" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="N52" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O52" s="6" t="n">
         <v>13.13</v>
@@ -4477,7 +4477,7 @@
         <v>177</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="K53" s="6" t="s">
         <v>43</v>
@@ -4486,10 +4486,10 @@
         <v>44</v>
       </c>
       <c r="M53" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="N53" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O53" s="6" t="n">
         <v>11.7</v>
@@ -4559,7 +4559,7 @@
         <v>181</v>
       </c>
       <c r="N55" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O55" s="6" t="n">
         <v>42.96</v>
@@ -4593,7 +4593,7 @@
         <v>190</v>
       </c>
       <c r="N56" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O56" s="6" t="n">
         <v>8.79</v>
@@ -4642,7 +4642,7 @@
         <v>57</v>
       </c>
       <c r="N57" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O57" s="6" t="n">
         <v>8.61</v>
@@ -4678,7 +4678,7 @@
         <v>57</v>
       </c>
       <c r="N58" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O58" s="6" t="n">
         <v>6.39</v>
@@ -4712,7 +4712,7 @@
         <v>57</v>
       </c>
       <c r="N59" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O59" s="6" t="n">
         <v>19.99</v>
@@ -4746,7 +4746,7 @@
         <v>57</v>
       </c>
       <c r="N60" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O60" s="6" t="n">
         <v>37.28</v>
@@ -4780,7 +4780,7 @@
         <v>57</v>
       </c>
       <c r="N61" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O61" s="6" t="n">
         <v>46.11</v>
@@ -4814,7 +4814,7 @@
         <v>207</v>
       </c>
       <c r="N62" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O62" s="6" t="n">
         <v>66452.74</v>
@@ -4886,7 +4886,7 @@
         <v>207</v>
       </c>
       <c r="N64" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O64" s="6" t="n">
         <v>0.01</v>
@@ -4922,7 +4922,7 @@
         <v>207</v>
       </c>
       <c r="N65" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O65" s="6" t="n">
         <v>0</v>
@@ -4958,7 +4958,7 @@
         <v>218</v>
       </c>
       <c r="N66" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O66" s="6" t="n">
         <v>0.42</v>
@@ -4996,7 +4996,7 @@
         <v>218</v>
       </c>
       <c r="N67" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O67" s="6" t="n">
         <v>0.71</v>
@@ -5034,7 +5034,7 @@
         <v>218</v>
       </c>
       <c r="N68" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O68" s="6" t="n">
         <v>0.03</v>
@@ -5072,7 +5072,7 @@
         <v>218</v>
       </c>
       <c r="N69" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O69" s="6" t="n">
         <v>0.28</v>
@@ -5110,7 +5110,7 @@
         <v>218</v>
       </c>
       <c r="N70" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O70" s="6" t="n">
         <v>0.71</v>
@@ -5148,7 +5148,7 @@
         <v>218</v>
       </c>
       <c r="N71" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O71" s="6" t="n">
         <v>0.19</v>
@@ -5186,7 +5186,7 @@
         <v>218</v>
       </c>
       <c r="N72" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O72" s="6" t="n">
         <v>0.33</v>
@@ -5224,7 +5224,7 @@
         <v>218</v>
       </c>
       <c r="N73" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O73" s="6" t="n">
         <v>0.75</v>
@@ -5262,7 +5262,7 @@
         <v>218</v>
       </c>
       <c r="N74" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O74" s="6" t="n">
         <v>0.04</v>
@@ -5300,7 +5300,7 @@
         <v>242</v>
       </c>
       <c r="N75" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O75" s="6" t="n">
         <v>0.06</v>
@@ -5335,7 +5335,7 @@
         <v>248</v>
       </c>
       <c r="N76" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O76" s="6" t="n">
         <v>39296898972.47</v>
@@ -5369,7 +5369,7 @@
         <v>248</v>
       </c>
       <c r="N77" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O77" s="6" t="n">
         <v>4486028684.18</v>
@@ -5403,7 +5403,7 @@
         <v>248</v>
       </c>
       <c r="N78" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O78" s="6" t="n">
         <v>8.76</v>
@@ -5589,7 +5589,7 @@
         <v>256</v>
       </c>
       <c r="N83" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O83" s="6" t="n">
         <v>6.9</v>
@@ -5627,7 +5627,7 @@
         <v>256</v>
       </c>
       <c r="N84" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O84" s="6" t="n">
         <v>29.15</v>
@@ -5665,7 +5665,7 @@
         <v>256</v>
       </c>
       <c r="N85" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O85" s="6" t="n">
         <v>11.68</v>
@@ -5703,7 +5703,7 @@
         <v>256</v>
       </c>
       <c r="N86" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O86" s="6" t="n">
         <v>0.96</v>
@@ -5741,7 +5741,7 @@
         <v>256</v>
       </c>
       <c r="N87" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O87" s="6" t="n">
         <v>0.68</v>
@@ -5779,7 +5779,7 @@
         <v>256</v>
       </c>
       <c r="N88" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O88" s="6" t="n">
         <v>0.91</v>
@@ -5855,7 +5855,7 @@
         <v>284</v>
       </c>
       <c r="N90" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O90" s="6" t="n">
         <v>10.65</v>
@@ -5893,7 +5893,7 @@
         <v>284</v>
       </c>
       <c r="N91" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O91" s="6" t="n">
         <v>0.93</v>
@@ -5969,7 +5969,7 @@
         <v>295</v>
       </c>
       <c r="N93" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O93" s="6" t="n">
         <v>13.13</v>
@@ -6007,7 +6007,7 @@
         <v>295</v>
       </c>
       <c r="N94" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O94" s="6" t="n">
         <v>0.92</v>
@@ -6083,7 +6083,7 @@
         <v>304</v>
       </c>
       <c r="N96" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O96" s="6" t="n">
         <v>5.97</v>
@@ -6121,7 +6121,7 @@
         <v>304</v>
       </c>
       <c r="N97" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O97" s="6" t="n">
         <v>0.96</v>
@@ -6197,7 +6197,7 @@
         <v>314</v>
       </c>
       <c r="N99" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O99" s="6" t="n">
         <v>11.42</v>
@@ -6235,7 +6235,7 @@
         <v>314</v>
       </c>
       <c r="N100" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O100" s="6" t="n">
         <v>0.92</v>
@@ -6311,7 +6311,7 @@
         <v>322</v>
       </c>
       <c r="N102" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O102" s="6" t="n">
         <v>9.96</v>
@@ -6349,7 +6349,7 @@
         <v>322</v>
       </c>
       <c r="N103" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O103" s="6" t="n">
         <v>0.94</v>
@@ -6425,7 +6425,7 @@
         <v>332</v>
       </c>
       <c r="N105" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O105" s="6" t="n">
         <v>24.18</v>
@@ -6463,7 +6463,7 @@
         <v>332</v>
       </c>
       <c r="N106" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O106" s="6" t="n">
         <v>0.75</v>
@@ -6501,7 +6501,7 @@
         <v>343</v>
       </c>
       <c r="N107" s="6" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="O107" s="6" t="n">
         <v>9691</v>
@@ -6539,7 +6539,7 @@
         <v>350</v>
       </c>
       <c r="N108" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O108" s="6" t="n">
         <v>54200</v>
@@ -6576,7 +6576,7 @@
         <v>350</v>
       </c>
       <c r="N109" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O109" s="6" t="n">
         <v>37500</v>
@@ -6613,7 +6613,7 @@
         <v>350</v>
       </c>
       <c r="N110" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O110" s="6" t="n">
         <v>16900</v>
@@ -6650,7 +6650,7 @@
         <v>350</v>
       </c>
       <c r="N111" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O111" s="6" t="n">
         <v>9400</v>
@@ -6687,7 +6687,7 @@
         <v>350</v>
       </c>
       <c r="N112" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O112" s="6" t="n">
         <v>43300</v>
@@ -6724,7 +6724,7 @@
         <v>350</v>
       </c>
       <c r="N113" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O113" s="6" t="n">
         <v>1600</v>
@@ -6761,7 +6761,7 @@
         <v>350</v>
       </c>
       <c r="N114" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O114" s="6" t="n">
         <v>5600</v>
@@ -6798,7 +6798,7 @@
         <v>350</v>
       </c>
       <c r="N115" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O115" s="6" t="n">
         <v>49000</v>
@@ -8683,7 +8683,7 @@
       </c>
       <c r="M166" s="6"/>
       <c r="N166" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O166" s="6" t="n">
         <v>586.4</v>
@@ -8716,7 +8716,7 @@
       </c>
       <c r="M167" s="6"/>
       <c r="N167" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O167" s="6" t="n">
         <v>409.2</v>
@@ -8749,7 +8749,7 @@
       </c>
       <c r="M168" s="6"/>
       <c r="N168" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O168" s="6" t="n">
         <v>177.2</v>
@@ -8782,7 +8782,7 @@
       </c>
       <c r="M169" s="6"/>
       <c r="N169" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O169" s="6" t="n">
         <v>23.6</v>
@@ -8815,7 +8815,7 @@
       </c>
       <c r="M170" s="6"/>
       <c r="N170" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O170" s="6" t="n">
         <v>24.4</v>
@@ -8847,7 +8847,7 @@
       </c>
       <c r="M171" s="6"/>
       <c r="N171" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O171" s="6" t="n">
         <v>42.2</v>
@@ -8879,7 +8879,7 @@
       </c>
       <c r="M172" s="6"/>
       <c r="N172" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O172" s="6" t="n">
         <v>34.4</v>
@@ -8911,7 +8911,7 @@
       </c>
       <c r="M173" s="6"/>
       <c r="N173" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O173" s="6" t="n">
         <v>26.6</v>
@@ -8943,7 +8943,7 @@
       </c>
       <c r="M174" s="6"/>
       <c r="N174" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O174" s="6" t="n">
         <v>510.8</v>
@@ -8975,7 +8975,7 @@
       </c>
       <c r="M175" s="6"/>
       <c r="N175" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O175" s="6" t="n">
         <v>27</v>
@@ -9078,7 +9078,7 @@
         <v>498</v>
       </c>
       <c r="N178" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O178" s="6" t="n">
         <v>39.5</v>
@@ -9109,7 +9109,7 @@
         <v>498</v>
       </c>
       <c r="N179" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O179" s="6" t="n">
         <v>4.15</v>
@@ -9143,7 +9143,7 @@
         <v>503</v>
       </c>
       <c r="N180" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O180" s="6" t="n">
         <v>13.3</v>
@@ -9177,7 +9177,7 @@
         <v>503</v>
       </c>
       <c r="N181" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O181" s="6" t="n">
         <v>14.7</v>
@@ -9211,7 +9211,7 @@
         <v>503</v>
       </c>
       <c r="N182" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O182" s="6" t="n">
         <v>14.5</v>
@@ -9245,7 +9245,7 @@
         <v>503</v>
       </c>
       <c r="N183" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O183" s="6" t="n">
         <v>15.2</v>
@@ -9279,7 +9279,7 @@
         <v>503</v>
       </c>
       <c r="N184" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O184" s="6" t="n">
         <v>35.4</v>
@@ -9313,7 +9313,7 @@
         <v>503</v>
       </c>
       <c r="N185" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O185" s="6" t="n">
         <v>15.8</v>
@@ -9345,7 +9345,7 @@
       </c>
       <c r="M186" s="6"/>
       <c r="N186" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O186" s="6" t="n">
         <v>22</v>
@@ -9377,7 +9377,7 @@
       </c>
       <c r="M187" s="6"/>
       <c r="N187" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O187" s="6" t="n">
         <v>20.58</v>
@@ -9411,7 +9411,7 @@
         <v>524</v>
       </c>
       <c r="N188" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O188" s="6" t="n">
         <v>1</v>
@@ -9446,7 +9446,7 @@
         <v>524</v>
       </c>
       <c r="N189" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O189" s="6" t="n">
         <v>1</v>
@@ -9481,7 +9481,7 @@
         <v>524</v>
       </c>
       <c r="N190" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O190" s="6" t="n">
         <v>1</v>
@@ -9516,7 +9516,7 @@
         <v>524</v>
       </c>
       <c r="N191" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O191" s="6" t="n">
         <v>0</v>
@@ -9551,7 +9551,7 @@
         <v>524</v>
       </c>
       <c r="N192" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O192" s="6" t="n">
         <v>1</v>
@@ -9831,7 +9831,7 @@
         <v>548</v>
       </c>
       <c r="N200" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O200" s="6" t="n">
         <v>1</v>
@@ -9866,7 +9866,7 @@
         <v>548</v>
       </c>
       <c r="N201" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O201" s="6" t="n">
         <v>0</v>
@@ -9997,7 +9997,7 @@
         <v>559</v>
       </c>
       <c r="N205" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O205" s="6" t="n">
         <v>1</v>
@@ -10029,7 +10029,7 @@
         <v>559</v>
       </c>
       <c r="N206" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O206" s="6" t="n">
         <v>1</v>
@@ -10061,7 +10061,7 @@
         <v>559</v>
       </c>
       <c r="N207" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="O207" s="6" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
fix typo: MsAsPdmpDt -> MsAcPdmpDt, found in #75
</commit_message>
<xml_diff>
--- a/data_final/dictionaries/S_Dict.xlsx
+++ b/data_final/dictionaries/S_Dict.xlsx
@@ -1614,7 +1614,7 @@
     <t xml:space="preserve">Fraction of year that state has a “modern system” operational and users could access (as determined by Horowitz et al., 2018).</t>
   </si>
   <si>
-    <t xml:space="preserve">MsAsPdmpFr</t>
+    <t xml:space="preserve">MsAcPdmpFr</t>
   </si>
   <si>
     <t xml:space="preserve">Fraction of year that state has any legislation requiring Prescribers to access PDMP before prescribing (as interpreted by PDAPS) enacted.</t>
@@ -2129,8 +2129,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ232"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A166" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H192" activeCellId="0" sqref="H192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>